<commit_message>
Update file Meeting 06/10
</commit_message>
<xml_diff>
--- a/CM_Plan/Management/Meeting/WLS_Project Meeting Minutes_06-10-2020.xlsx
+++ b/CM_Plan/Management/Meeting/WLS_Project Meeting Minutes_06-10-2020.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="92">
   <si>
     <t>MEETING MINUTES</t>
   </si>
@@ -299,7 +299,10 @@
     <t>+ Thiếu Product Meeting mặc định.</t>
   </si>
   <si>
-    <t>+ Làm rõ, xử lý Create-Edit-Update</t>
+    <t>+ Thiếu Product Meeting mặc định. =&gt; Ý 21</t>
+  </si>
+  <si>
+    <t>+ Làm rõ, xử lý chức năng Create-Edit-Test =&gt; Ý 6</t>
   </si>
   <si>
     <t>+ Database :</t>
@@ -330,8 +333,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -389,9 +392,69 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -404,29 +467,52 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -440,89 +526,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="Tahoma"/>
       <charset val="1"/>
@@ -549,13 +552,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -567,169 +732,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -795,35 +798,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -843,6 +822,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -854,21 +848,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -892,127 +871,151 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1021,19 +1024,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1465,8 +1468,8 @@
   <sheetPr/>
   <dimension ref="A2:I109"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4533333333333" defaultRowHeight="15" customHeight="1"/>
@@ -2120,8 +2123,8 @@
   <sheetPr/>
   <dimension ref="D3:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="O57" sqref="O57"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75" outlineLevelCol="4"/>
@@ -2356,12 +2359,12 @@
     </row>
     <row r="60" spans="4:4">
       <c r="D60" s="31" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="4:4">
       <c r="D61" s="31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2383,37 +2386,37 @@
   <sheetData>
     <row r="6" spans="4:4">
       <c r="D6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="4:4">
       <c r="D8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="4:4">
       <c r="D9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="4:4">
       <c r="D11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="4:4">
       <c r="D12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="4:4">
       <c r="D14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="4:4">
       <c r="D15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>